<commit_message>
Standard Positive Control List updated for Yfiler Plus
</commit_message>
<xml_diff>
--- a/osiris/Documentation/StandardPositiveControlList.xlsx
+++ b/osiris/Documentation/StandardPositiveControlList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="115">
   <si>
     <t>Locus</t>
   </si>
@@ -351,6 +351,24 @@
   </si>
   <si>
     <t>DNA007</t>
+  </si>
+  <si>
+    <t>DYS627</t>
+  </si>
+  <si>
+    <t>DYS460</t>
+  </si>
+  <si>
+    <t>DYS518</t>
+  </si>
+  <si>
+    <t>DYS449</t>
+  </si>
+  <si>
+    <t>DYF387S1</t>
+  </si>
+  <si>
+    <t>35,37</t>
   </si>
 </sst>
 </file>
@@ -671,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1199,6 +1217,9 @@
       <c r="C28" s="1">
         <v>16</v>
       </c>
+      <c r="E28" s="1">
+        <v>19</v>
+      </c>
       <c r="F28" s="1">
         <v>18</v>
       </c>
@@ -1378,6 +1399,9 @@
       <c r="C41" s="1">
         <v>24</v>
       </c>
+      <c r="E41" s="1">
+        <v>22</v>
+      </c>
       <c r="F41" s="1">
         <v>22</v>
       </c>
@@ -1400,6 +1424,9 @@
       <c r="C43" s="1">
         <v>12</v>
       </c>
+      <c r="E43" s="1">
+        <v>13</v>
+      </c>
       <c r="F43" s="1">
         <v>12</v>
       </c>
@@ -1477,6 +1504,46 @@
       </c>
       <c r="E49" s="1">
         <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>109</v>
+      </c>
+      <c r="E50" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>110</v>
+      </c>
+      <c r="E51" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>111</v>
+      </c>
+      <c r="E52" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>112</v>
+      </c>
+      <c r="E53" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>113</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed font to make more readable
</commit_message>
<xml_diff>
--- a/osiris/Documentation/StandardPositiveControlList.xlsx
+++ b/osiris/Documentation/StandardPositiveControlList.xlsx
@@ -375,9 +375,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -404,9 +411,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -691,858 +699,860 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="6" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="6" width="8.88671875" style="2"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C1" s="2">
         <v>9948</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="2">
         <v>16</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="2">
         <v>11</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="2">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="2">
         <v>1</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="2">
         <v>9.3000000000000007</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="2">
         <v>8</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="2">
         <v>8</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="2">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="2">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="2">
         <v>11</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="2">
         <v>17</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="2">
         <v>16</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="2">
         <v>13</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="2">
         <v>12</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="2">
         <v>30</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="2">
         <v>11</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="2">
         <v>11</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="2">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="2">
         <v>11</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="2">
         <v>11</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="2">
         <v>8</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="2">
         <v>11</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="2">
         <v>23</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="2">
         <v>17</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" s="2" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F18" s="2" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19" s="2">
         <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F20" s="2" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="2">
         <v>18.3</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F21" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="2">
         <v>23</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F22" s="2" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="A23" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F23" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="A24" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="2">
         <v>11</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F24" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="A25" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="2">
         <v>12</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F25" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="A26" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="2">
         <v>12</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F26" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="A27" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="2">
         <v>10</v>
       </c>
-      <c r="E27" s="1">
+      <c r="E27" s="2">
         <v>11</v>
       </c>
-      <c r="F27" s="1">
+      <c r="F27" s="2">
         <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="A28" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" s="2">
         <v>16</v>
       </c>
-      <c r="E28" s="1">
+      <c r="E28" s="2">
         <v>19</v>
       </c>
-      <c r="F28" s="1">
+      <c r="F28" s="2">
         <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="A29" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29" s="2">
         <v>18</v>
       </c>
-      <c r="E29" s="1">
+      <c r="E29" s="2">
         <v>17</v>
       </c>
-      <c r="F29" s="1">
+      <c r="F29" s="2">
         <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="A30" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="2">
         <v>13</v>
       </c>
-      <c r="E30" s="1">
+      <c r="E30" s="2">
         <v>13</v>
       </c>
-      <c r="F30" s="1">
+      <c r="F30" s="2">
         <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="A31" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="2">
         <v>12</v>
       </c>
-      <c r="E31" s="1">
+      <c r="E31" s="2">
         <v>12</v>
       </c>
-      <c r="F31" s="1">
+      <c r="F31" s="2">
         <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="A32" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C32" s="2">
         <v>31</v>
       </c>
-      <c r="E32" s="1">
+      <c r="E32" s="2">
         <v>29</v>
       </c>
-      <c r="F32" s="1">
+      <c r="F32" s="2">
         <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="A33" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="2">
         <v>11</v>
       </c>
-      <c r="E33" s="1">
+      <c r="E33" s="2">
         <v>12</v>
       </c>
-      <c r="F33" s="1">
+      <c r="F33" s="2">
         <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+      <c r="A34" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C34" s="2">
         <v>15</v>
       </c>
-      <c r="E34" s="1">
+      <c r="E34" s="2">
         <v>15</v>
       </c>
-      <c r="F34" s="1">
+      <c r="F34" s="2">
         <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+      <c r="A35" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35" s="2">
         <v>14</v>
       </c>
-      <c r="E35" s="1">
+      <c r="E35" s="2">
         <v>15</v>
       </c>
-      <c r="F35" s="1">
+      <c r="F35" s="2">
         <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+      <c r="A36" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" s="2">
         <v>13</v>
       </c>
-      <c r="E36" s="1">
+      <c r="E36" s="2">
         <v>13</v>
       </c>
-      <c r="F36" s="1">
+      <c r="F36" s="2">
         <v>13</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+      <c r="A37" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C37" s="2">
         <v>13</v>
       </c>
-      <c r="E37" s="1">
+      <c r="E37" s="2">
         <v>13</v>
       </c>
-      <c r="F37" s="1">
+      <c r="F37" s="2">
         <v>13</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+      <c r="A38" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C38" s="2">
         <v>24</v>
       </c>
-      <c r="E38" s="1">
+      <c r="E38" s="2">
         <v>24</v>
       </c>
-      <c r="F38" s="1">
+      <c r="F38" s="2">
         <v>24</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+      <c r="A39" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E39" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="F39" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+      <c r="A40" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C40" s="1">
+      <c r="C40" s="2">
         <v>19</v>
       </c>
-      <c r="E40" s="1">
+      <c r="E40" s="2">
         <v>19</v>
       </c>
-      <c r="F40" s="1">
+      <c r="F40" s="2">
         <v>19</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+      <c r="A41" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C41" s="1">
+      <c r="C41" s="2">
         <v>24</v>
       </c>
-      <c r="E41" s="1">
+      <c r="E41" s="2">
         <v>22</v>
       </c>
-      <c r="F41" s="1">
+      <c r="F41" s="2">
         <v>22</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+      <c r="A42" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C42" s="2">
         <v>13</v>
       </c>
-      <c r="F42" s="1">
+      <c r="F42" s="2">
         <v>13</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+      <c r="A43" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43" s="2">
         <v>12</v>
       </c>
-      <c r="E43" s="1">
+      <c r="E43" s="2">
         <v>13</v>
       </c>
-      <c r="F43" s="1">
+      <c r="F43" s="2">
         <v>12</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+      <c r="A44" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C44" s="2">
         <v>23</v>
       </c>
-      <c r="E44" s="1">
+      <c r="E44" s="2">
         <v>24</v>
       </c>
-      <c r="F44" s="1">
+      <c r="F44" s="2">
         <v>21</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+      <c r="A45" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C45" s="2">
         <v>11</v>
       </c>
-      <c r="F45" s="1">
+      <c r="F45" s="2">
         <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+      <c r="A46" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C46" s="2">
         <v>18</v>
       </c>
-      <c r="E46" s="1">
+      <c r="E46" s="2">
         <v>17</v>
       </c>
-      <c r="F46" s="1">
+      <c r="F46" s="2">
         <v>17</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+      <c r="A47" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C47" s="2">
         <v>17</v>
       </c>
-      <c r="E47" s="1">
+      <c r="E47" s="2">
         <v>15</v>
       </c>
-      <c r="F47" s="1">
+      <c r="F47" s="2">
         <v>17</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+      <c r="A48" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C48" s="1">
+      <c r="C48" s="2">
         <v>12</v>
       </c>
-      <c r="E48" s="1">
+      <c r="E48" s="2">
         <v>13</v>
       </c>
-      <c r="F48" s="1">
+      <c r="F48" s="2">
         <v>11</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+      <c r="A49" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E49" s="1">
+      <c r="E49" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+      <c r="A50" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E50" s="1">
+      <c r="E50" s="2">
         <v>21</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+      <c r="A51" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E51" s="1">
+      <c r="E51" s="2">
         <v>11</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+      <c r="A52" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E52" s="1">
+      <c r="E52" s="2">
         <v>37</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+      <c r="A53" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E53" s="1">
+      <c r="E53" s="2">
         <v>30</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+      <c r="A54" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="E54" s="1" t="s">
+      <c r="E54" s="2" t="s">
         <v>114</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added QS1 and QS2 for Qiagen 24plex
</commit_message>
<xml_diff>
--- a/osiris/Documentation/StandardPositiveControlList.xlsx
+++ b/osiris/Documentation/StandardPositiveControlList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="117">
   <si>
     <t>Locus</t>
   </si>
@@ -369,6 +369,12 @@
   </si>
   <si>
     <t>35,37</t>
+  </si>
+  <si>
+    <t>QS1</t>
+  </si>
+  <si>
+    <t>QS2</t>
   </si>
 </sst>
 </file>
@@ -697,10 +703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F54"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1508,7 +1514,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>99</v>
       </c>
@@ -1516,7 +1522,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>109</v>
       </c>
@@ -1524,7 +1530,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>110</v>
       </c>
@@ -1532,7 +1538,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>111</v>
       </c>
@@ -1540,7 +1546,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>112</v>
       </c>
@@ -1548,12 +1554,52 @@
         <v>30</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>113</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>114</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B55" s="2">
+        <v>1</v>
+      </c>
+      <c r="C55" s="2">
+        <v>1</v>
+      </c>
+      <c r="D55" s="2">
+        <v>1</v>
+      </c>
+      <c r="E55" s="2">
+        <v>1</v>
+      </c>
+      <c r="F55" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B56" s="2">
+        <v>2</v>
+      </c>
+      <c r="C56" s="2">
+        <v>2</v>
+      </c>
+      <c r="D56" s="2">
+        <v>2</v>
+      </c>
+      <c r="E56" s="2">
+        <v>2</v>
+      </c>
+      <c r="F56" s="2">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added loci and control for Qiagen Argus X-12 kit
</commit_message>
<xml_diff>
--- a/osiris/Documentation/StandardPositiveControlList.xlsx
+++ b/osiris/Documentation/StandardPositiveControlList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="133">
   <si>
     <t>Locus</t>
   </si>
@@ -375,6 +375,54 @@
   </si>
   <si>
     <t>QS2</t>
+  </si>
+  <si>
+    <t>DXS7132</t>
+  </si>
+  <si>
+    <t>DXS7423</t>
+  </si>
+  <si>
+    <t>DXS8378</t>
+  </si>
+  <si>
+    <t>DXS10074</t>
+  </si>
+  <si>
+    <t>DXS10079</t>
+  </si>
+  <si>
+    <t>DXS10101</t>
+  </si>
+  <si>
+    <t>DXS10103</t>
+  </si>
+  <si>
+    <t>DXS10134</t>
+  </si>
+  <si>
+    <t>DXS10135</t>
+  </si>
+  <si>
+    <t>DXS10146</t>
+  </si>
+  <si>
+    <t>DXS10148</t>
+  </si>
+  <si>
+    <t>HPRTB</t>
+  </si>
+  <si>
+    <t>30,31</t>
+  </si>
+  <si>
+    <t>35,36</t>
+  </si>
+  <si>
+    <t>21.1,27</t>
+  </si>
+  <si>
+    <t>22.1,23.1</t>
   </si>
 </sst>
 </file>
@@ -703,20 +751,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I63" sqref="I63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="6" width="8.88671875" style="2"/>
-    <col min="7" max="16384" width="8.88671875" style="1"/>
+    <col min="2" max="7" width="8.88671875" style="2"/>
+    <col min="8" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -735,8 +783,11 @@
       <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" s="2">
+        <v>3657</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -756,7 +807,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -776,7 +827,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -795,8 +846,11 @@
       <c r="F4" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>104</v>
       </c>
@@ -816,7 +870,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -836,7 +890,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -856,7 +910,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -876,7 +930,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
@@ -896,7 +950,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -916,7 +970,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
@@ -936,7 +990,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
@@ -956,7 +1010,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -976,7 +1030,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
@@ -996,7 +1050,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>27</v>
       </c>
@@ -1016,7 +1070,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>33</v>
       </c>
@@ -1514,7 +1568,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>99</v>
       </c>
@@ -1522,7 +1576,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>109</v>
       </c>
@@ -1530,7 +1584,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>110</v>
       </c>
@@ -1538,7 +1592,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>111</v>
       </c>
@@ -1546,7 +1600,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>112</v>
       </c>
@@ -1554,7 +1608,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>113</v>
       </c>
@@ -1562,7 +1616,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>115</v>
       </c>
@@ -1582,7 +1636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>116</v>
       </c>
@@ -1600,6 +1654,210 @@
       </c>
       <c r="F56" s="2">
         <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B57" s="2">
+        <v>12</v>
+      </c>
+      <c r="C57" s="2">
+        <v>13</v>
+      </c>
+      <c r="D57" s="2">
+        <v>13</v>
+      </c>
+      <c r="G57" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C58" s="2">
+        <v>14</v>
+      </c>
+      <c r="D58" s="2">
+        <v>17</v>
+      </c>
+      <c r="G58" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C59" s="2">
+        <v>11</v>
+      </c>
+      <c r="D59" s="2">
+        <v>10</v>
+      </c>
+      <c r="G59" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C60" s="2">
+        <v>18</v>
+      </c>
+      <c r="D60" s="2">
+        <v>17</v>
+      </c>
+      <c r="G60" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C61" s="2">
+        <v>19</v>
+      </c>
+      <c r="D61" s="2">
+        <v>17</v>
+      </c>
+      <c r="G61" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C62" s="2">
+        <v>32</v>
+      </c>
+      <c r="D62" s="2">
+        <v>31</v>
+      </c>
+      <c r="G62" s="2">
+        <v>29.2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B63" s="2">
+        <v>17</v>
+      </c>
+      <c r="C63" s="2">
+        <v>18</v>
+      </c>
+      <c r="D63" s="2">
+        <v>17</v>
+      </c>
+      <c r="G63" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C64" s="2">
+        <v>34</v>
+      </c>
+      <c r="D64" s="2">
+        <v>32</v>
+      </c>
+      <c r="G64" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C65" s="2">
+        <v>22</v>
+      </c>
+      <c r="D65" s="2">
+        <v>27</v>
+      </c>
+      <c r="G65" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B66" s="2">
+        <v>28</v>
+      </c>
+      <c r="C66" s="2">
+        <v>29</v>
+      </c>
+      <c r="D66" s="2">
+        <v>29</v>
+      </c>
+      <c r="G66" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C67" s="2">
+        <v>23</v>
+      </c>
+      <c r="D67" s="2">
+        <v>23.1</v>
+      </c>
+      <c r="G67" s="2">
+        <v>23.1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B68" s="2">
+        <v>14</v>
+      </c>
+      <c r="C68" s="2">
+        <v>14</v>
+      </c>
+      <c r="D68" s="2">
+        <v>13</v>
+      </c>
+      <c r="G68" s="2">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated GenerateLadderFile.vcxproj and added to TestAnalysis.sln
</commit_message>
<xml_diff>
--- a/osiris/Documentation/StandardPositiveControlList.xlsx
+++ b/osiris/Documentation/StandardPositiveControlList.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goorrob\Documents\GitHub\osiris\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{27188706-97D0-4CAB-B1F8-C7C29972233B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21432" windowHeight="11172"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21435" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="139">
   <si>
     <t>Locus</t>
   </si>
@@ -423,12 +424,30 @@
   </si>
   <si>
     <t>22.1,23.1</t>
+  </si>
+  <si>
+    <t>MK1</t>
+  </si>
+  <si>
+    <t>14,17.3</t>
+  </si>
+  <si>
+    <t>21,23</t>
+  </si>
+  <si>
+    <t>20,22.2</t>
+  </si>
+  <si>
+    <t>9,12</t>
+  </si>
+  <si>
+    <t>24.2,29.2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -750,21 +769,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G68"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I63" sqref="I63"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="7" width="8.88671875" style="2"/>
-    <col min="8" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="8" width="8.85546875" style="2"/>
+    <col min="9" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -786,8 +805,11 @@
       <c r="G1" s="2">
         <v>3657</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -806,8 +828,11 @@
       <c r="F2" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -826,8 +851,11 @@
       <c r="F3" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H3" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -849,8 +877,11 @@
       <c r="G4" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H4" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>104</v>
       </c>
@@ -869,8 +900,11 @@
       <c r="F5" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H5" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -889,8 +923,11 @@
       <c r="F6" s="2">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -909,8 +946,11 @@
       <c r="F7" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H7" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -929,8 +969,11 @@
       <c r="F8" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H8" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
@@ -949,8 +992,11 @@
       <c r="F9" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H9" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -969,8 +1015,11 @@
       <c r="F10" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H10" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
@@ -989,8 +1038,11 @@
       <c r="F11" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H11" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
@@ -1009,8 +1061,11 @@
       <c r="F12" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H12" s="2">
+        <v>30.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -1029,8 +1084,11 @@
       <c r="F13" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H13" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
@@ -1049,8 +1107,11 @@
       <c r="F14" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H14" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>27</v>
       </c>
@@ -1069,8 +1130,11 @@
       <c r="F15" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H15" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>33</v>
       </c>
@@ -1090,7 +1154,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>35</v>
       </c>
@@ -1110,7 +1174,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>43</v>
       </c>
@@ -1126,8 +1190,11 @@
       <c r="F18" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H18" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>45</v>
       </c>
@@ -1143,8 +1210,11 @@
       <c r="F19" s="2">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H19" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>48</v>
       </c>
@@ -1160,8 +1230,11 @@
       <c r="F20" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H20" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>50</v>
       </c>
@@ -1177,8 +1250,11 @@
       <c r="F21" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H21" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>52</v>
       </c>
@@ -1197,8 +1273,11 @@
       <c r="F22" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H22" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>54</v>
       </c>
@@ -1214,8 +1293,11 @@
       <c r="F23" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H23" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>56</v>
       </c>
@@ -1232,7 +1314,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>57</v>
       </c>
@@ -1252,7 +1334,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>71</v>
       </c>
@@ -1266,7 +1348,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>76</v>
       </c>
@@ -1280,7 +1362,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>77</v>
       </c>
@@ -1294,7 +1376,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>78</v>
       </c>
@@ -1308,7 +1390,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>79</v>
       </c>
@@ -1322,7 +1404,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>80</v>
       </c>
@@ -1336,7 +1418,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>81</v>
       </c>
@@ -1350,7 +1432,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>82</v>
       </c>
@@ -1364,7 +1446,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>83</v>
       </c>
@@ -1378,7 +1460,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>84</v>
       </c>
@@ -1392,7 +1474,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>85</v>
       </c>
@@ -1406,7 +1488,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>86</v>
       </c>
@@ -1420,7 +1502,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>87</v>
       </c>
@@ -1434,7 +1516,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>88</v>
       </c>
@@ -1448,7 +1530,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>90</v>
       </c>
@@ -1462,7 +1544,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>91</v>
       </c>
@@ -1476,7 +1558,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>92</v>
       </c>
@@ -1487,7 +1569,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>93</v>
       </c>
@@ -1501,7 +1583,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>94</v>
       </c>
@@ -1515,7 +1597,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>95</v>
       </c>
@@ -1526,7 +1608,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>96</v>
       </c>
@@ -1540,7 +1622,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>97</v>
       </c>
@@ -1554,7 +1636,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>98</v>
       </c>
@@ -1568,7 +1650,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>99</v>
       </c>
@@ -1576,7 +1658,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>109</v>
       </c>
@@ -1584,7 +1666,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>110</v>
       </c>
@@ -1592,7 +1674,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>111</v>
       </c>
@@ -1600,7 +1682,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>112</v>
       </c>
@@ -1608,7 +1690,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>113</v>
       </c>
@@ -1616,7 +1698,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>115</v>
       </c>
@@ -1636,7 +1718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>116</v>
       </c>
@@ -1656,7 +1738,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>117</v>
       </c>
@@ -1673,7 +1755,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>118</v>
       </c>
@@ -1690,7 +1772,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>119</v>
       </c>
@@ -1707,7 +1789,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>120</v>
       </c>
@@ -1724,7 +1806,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>121</v>
       </c>
@@ -1741,7 +1823,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>122</v>
       </c>
@@ -1758,7 +1840,7 @@
         <v>29.2</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>123</v>
       </c>
@@ -1775,7 +1857,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>124</v>
       </c>
@@ -1792,7 +1874,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>125</v>
       </c>
@@ -1809,7 +1891,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>126</v>
       </c>
@@ -1826,7 +1908,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>127</v>
       </c>
@@ -1843,7 +1925,7 @@
         <v>23.1</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>128</v>
       </c>

</xml_diff>